<commit_message>
password and minor formatting changes
</commit_message>
<xml_diff>
--- a/heatmap_offices.xlsx
+++ b/heatmap_offices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cadenlin/PycharmProjects/heatmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F4E3F4-A727-5947-B0F4-21AF23CC928D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A928920-797F-0D45-8D6B-F33226CBCD6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49280" yWindow="480" windowWidth="17920" windowHeight="21120" activeTab="7" xr2:uid="{D5E28685-1826-2A4E-99D6-346D44856473}"/>
+    <workbookView xWindow="28820" yWindow="500" windowWidth="18320" windowHeight="21100" activeTab="7" xr2:uid="{D5E28685-1826-2A4E-99D6-346D44856473}"/>
   </bookViews>
   <sheets>
     <sheet name="McCain" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>lat</t>
   </si>
@@ -57,15 +57,9 @@
     <t>comments</t>
   </si>
   <si>
-    <t>Vista, CA</t>
-  </si>
-  <si>
     <t>Manufacturing facility</t>
   </si>
   <si>
-    <t>Headquarters and manufacturing facility</t>
-  </si>
-  <si>
     <t>Regional office</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>Fremont, CA</t>
   </si>
   <si>
-    <t>Anaheim, CA</t>
-  </si>
-  <si>
     <t>Santa Fe, CA</t>
   </si>
   <si>
@@ -153,24 +144,9 @@
     <t>Souderton, PA</t>
   </si>
   <si>
-    <t>Decatur, AL</t>
-  </si>
-  <si>
-    <t>Headquarters</t>
-  </si>
-  <si>
-    <t>Chesapeake, VA</t>
-  </si>
-  <si>
     <t>Tucson, AZ</t>
   </si>
   <si>
-    <t>San Diego, CA</t>
-  </si>
-  <si>
-    <t>Pflugerville, TX</t>
-  </si>
-  <si>
     <t>Davenport, IA</t>
   </si>
   <si>
@@ -178,9 +154,6 @@
   </si>
   <si>
     <t>Volo, IL</t>
-  </si>
-  <si>
-    <t>Everett, WA</t>
   </si>
 </sst>
 </file>
@@ -540,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC36596-AA2E-594D-8534-B720AB1EB71E}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,20 +535,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="B2">
-        <v>-117.24250000000001</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -583,10 +542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6F68AE-C9EA-1646-9FBE-6D3EAD8BEC19}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,10 +575,10 @@
         <v>-122.771933</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -630,10 +589,10 @@
         <v>-122.15607679999999</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -644,262 +603,248 @@
         <v>-121.98857099999999</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>33.834751599999997</v>
+        <v>37.177889</v>
       </c>
       <c r="B5">
-        <v>-117.911732</v>
+        <v>-99.771434999999997</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>37.177889</v>
+        <v>34.4635757</v>
       </c>
       <c r="B6">
-        <v>-99.771434999999997</v>
+        <v>-113.41577150000001</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>34.4635757</v>
+        <v>32.735581600000003</v>
       </c>
       <c r="B7">
-        <v>-113.41577150000001</v>
+        <v>-97.107118600000007</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>32.735581600000003</v>
+        <v>29.758938199999999</v>
       </c>
       <c r="B8">
-        <v>-97.107118600000007</v>
+        <v>-95.367697399999997</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>29.758938199999999</v>
+        <v>41.732079599999999</v>
       </c>
       <c r="B9">
-        <v>-95.367697399999997</v>
+        <v>-93.605091999999999</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>41.732079599999999</v>
+        <v>45.031355900000001</v>
       </c>
       <c r="B10">
-        <v>-93.605091999999999</v>
+        <v>-92.792984200000006</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>45.031355900000001</v>
+        <v>47.620100499999999</v>
       </c>
       <c r="B11">
-        <v>-92.792984200000006</v>
+        <v>-92.436334299999999</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>47.620100499999999</v>
+        <v>41.7563344</v>
       </c>
       <c r="B12">
-        <v>-92.436334299999999</v>
+        <v>-88.045558999999997</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>41.7563344</v>
+        <v>36.1622767</v>
       </c>
       <c r="B13">
-        <v>-88.045558999999997</v>
+        <v>-86.774298400000006</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>36.1622767</v>
+        <v>42.485312499999999</v>
       </c>
       <c r="B14">
-        <v>-86.774298400000006</v>
+        <v>-83.377155299999998</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>42.485312499999999</v>
+        <v>41.312555199999998</v>
       </c>
       <c r="B15">
-        <v>-83.377155299999998</v>
+        <v>-81.440112900000003</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>41.312555199999998</v>
+        <v>34.0709576</v>
       </c>
       <c r="B16">
-        <v>-81.440112900000003</v>
+        <v>-84.274732900000004</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>34.0709576</v>
+        <v>34.924866700000003</v>
       </c>
       <c r="B17">
-        <v>-84.274732900000004</v>
+        <v>-81.025078399999998</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>34.924866700000003</v>
+        <v>37.538508700000001</v>
       </c>
       <c r="B18">
-        <v>-81.025078399999998</v>
+        <v>-77.434280000000001</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>37.538508700000001</v>
+        <v>39.1648</v>
       </c>
       <c r="B19">
-        <v>-77.434280000000001</v>
+        <v>-76.624943700000003</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>39.1648</v>
+        <v>40.568824499999998</v>
       </c>
       <c r="B20">
-        <v>-76.624943700000003</v>
+        <v>-74.700273889745063</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>40.568824499999998</v>
+        <v>40.311770699999997</v>
       </c>
       <c r="B21">
-        <v>-74.700273889745063</v>
+        <v>-75.325175900000005</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>40.311770699999997</v>
-      </c>
-      <c r="B22">
-        <v>-75.325175900000005</v>
-      </c>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +855,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B901D917-9A8F-1B43-90EA-4F7F1874FE53}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,20 +877,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>34.605899999999998</v>
-      </c>
-      <c r="B2">
-        <v>-86.9833</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -953,10 +884,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196C5471-B6DF-9B4A-95DE-B9AB656C7783}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,30 +908,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>36.7682</v>
+        <v>32.253999999999998</v>
       </c>
       <c r="B2">
-        <v>-76.287499999999994</v>
+        <v>-110.9742</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>32.253999999999998</v>
-      </c>
-      <c r="B3">
-        <v>-110.9742</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1010,10 +927,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCA8E0F-C1E8-1B47-8E21-A60D39FFFD3F}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,20 +949,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>29.760400000000001</v>
-      </c>
-      <c r="B2">
-        <v>-95.369799999999998</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1053,10 +956,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50605E5F-3FE2-CB49-B072-E80CB5628481}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,20 +978,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>32.715699999999998</v>
-      </c>
-      <c r="B2">
-        <v>-117.1611</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1096,10 +985,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F6A90-7F9C-6645-916B-4D89793EF430}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1123,58 +1012,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>30.439369599999999</v>
+        <v>41.523580799999998</v>
       </c>
       <c r="B2">
-        <v>-97.620004300000005</v>
+        <v>-90.577096699999998</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>41.523580799999998</v>
+        <v>37.553162200000003</v>
       </c>
       <c r="B3">
-        <v>-90.577096699999998</v>
+        <v>-77.911265499999999</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>37.553162200000003</v>
+        <v>42.326133200000001</v>
       </c>
       <c r="B4">
-        <v>-77.911265499999999</v>
+        <v>-88.167861000000002</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>42.326133200000001</v>
-      </c>
-      <c r="B5">
-        <v>-88.167861000000002</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1185,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497835E3-D2B9-0B49-9776-86091A698DBA}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:F25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1207,20 +1082,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>47.978999999999999</v>
-      </c>
-      <c r="B2">
-        <v>-122.2021</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>